<commit_message>
[Justice Counts][Ingest][4/n] Small fixes + infer aggregate values if flag is set (Recidiviz/recidiviz-data#14326)
GitOrigin-RevId: 1592cfc493fc6890174a9fd04358174f44d98465
</commit_message>
<xml_diff>
--- a/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/supervision/supervision_metrics.xlsx
+++ b/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/supervision/supervision_metrics.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/supervision/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945BFC06-CF36-3046-AAFB-B5B9870D1EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DC4505-1621-9A48-A237-A92AD5CB8B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8340" yWindow="2900" windowWidth="27640" windowHeight="16940" xr2:uid="{5617EF7D-61A0-204E-8417-5DBEB9B0F97B}"/>
+    <workbookView xWindow="8340" yWindow="2900" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{5617EF7D-61A0-204E-8417-5DBEB9B0F97B}"/>
   </bookViews>
   <sheets>
     <sheet name="annual_budget" sheetId="1" r:id="rId1"/>
+    <sheet name="total_staff" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>year</t>
   </si>
@@ -53,6 +54,15 @@
   </si>
   <si>
     <t>probation</t>
+  </si>
+  <si>
+    <t>staff_type</t>
+  </si>
+  <si>
+    <t>SUPPORT</t>
+  </si>
+  <si>
+    <t>SUPERVISION</t>
   </si>
 </sst>
 </file>
@@ -406,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7985959D-817F-6F4A-8BD0-4153284D83EC}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -470,4 +480,61 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB61EDD-B3D3-2A41-8482-7B0B4AB84F2F}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2021</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2021</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Justice Counts][2/n] Get rid of "All" value in Tech Spec (Recidiviz/recidiviz-data#14533)
GitOrigin-RevId: bd43bdbeb70b422cb4269ea52b8f89261178ba78
</commit_message>
<xml_diff>
--- a/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/supervision/supervision_metrics.xlsx
+++ b/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/supervision/supervision_metrics.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilidworkin/recidiviz/recidiviz-data/recidiviz/tests/justice_counts/bulk_upload/bulk_upload_fixtures/supervision/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DC4505-1621-9A48-A237-A92AD5CB8B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A12CE3-CF28-0F47-85CB-9C6C337DF828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8340" yWindow="2900" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{5617EF7D-61A0-204E-8417-5DBEB9B0F97B}"/>
+    <workbookView xWindow="52940" yWindow="2120" windowWidth="18220" windowHeight="15340" activeTab="1" xr2:uid="{5617EF7D-61A0-204E-8417-5DBEB9B0F97B}"/>
   </bookViews>
   <sheets>
     <sheet name="annual_budget" sheetId="1" r:id="rId1"/>
-    <sheet name="total_staff" sheetId="2" r:id="rId2"/>
+    <sheet name="total_staff_by_type" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -487,7 +487,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>